<commit_message>
Made changes to the Market survey RAP using sqlite.
</commit_message>
<xml_diff>
--- a/data/open/MS1_Classification.xlsx
+++ b/data/open/MS1_Classification.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataViz\MS\vnso-RAP-marketStats-materials\data\open\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataViz\Market Survey\vnso-RAP-marketStats-materials\data\open\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="staple_type" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>